<commit_message>
up to wide and long data
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{0F11F1AA-B606-984E-9256-227C29A5546E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4A2C1F0-9D1E-7F40-92FC-6AEFC377875E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="3" xr2:uid="{5EADE905-632C-A04D-8302-0650934DE955}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{5EADE905-632C-A04D-8302-0650934DE955}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86BCBFC-8BEB-CC49-B231-5F3C6569F554}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1830,7 +1830,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2369,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8F7AE2-45CB-5144-B993-E6D0AB0BEE80}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>